<commit_message>
Auto update Excel log
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -629,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5272,6 +5272,582 @@
         </is>
       </c>
       <c r="F145" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>11:58:34</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>11:58:39</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:58:44</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:58:49</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>11:58:54</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>11:58:58</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:02:50</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:02:55</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>12:03:00</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>12:03:05</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>12:03:10</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>12:03:15</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>12:03:20</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>12:03:25</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>12:03:30</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>12:03:35</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>12:03:40</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>12:03:45</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -5288,7 +5864,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9547,6 +10123,646 @@
         </is>
       </c>
       <c r="F133" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:58:33</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>88.3%</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:58:37</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>88.3%</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11:58:41</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>87.4%</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>11:58:45</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>88.3%</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:58:53</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>87.4%</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:58:57</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>88.4%</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:59:01</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>87.4%</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>12:02:50</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>88.0%</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>12:02:54</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>87.9%</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>12:03:02</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>87.9%</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>12:03:06</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>87.0%</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:03:10</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>87.9%</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>12:03:14</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>87.9%</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>12:03:18</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>87.9%</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>12:03:26</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>87.0%</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>12:03:30</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>88.0%</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>12:03:34</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>88.0%</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>12:03:38</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>87.0%</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:03:42</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>88.0%</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:03:47</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>87.1%</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -9563,7 +10779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13822,6 +15038,646 @@
         </is>
       </c>
       <c r="F133" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>11:58:33</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>11:58:37</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>11:58:41</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>11:58:45</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:58:53</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:58:57</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:59:01</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>22.9C</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>12:02:51</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>12:02:55</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>12:03:03</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>12:03:07</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>12:03:11</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>12:03:15</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>12:03:19</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>12:03:27</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>12:03:31</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>12:03:35</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>12:03:39</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>12:03:43</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>12:03:47</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>23.0C</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:04:14
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1487,6 +1487,358 @@
         </is>
       </c>
       <c r="F30" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:03:13</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:03:18</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:03:23</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:03:30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:03:35</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:03:40</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:03:45</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:03:49</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>14:03:57</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:04:02</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>14:04:04</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -1503,7 +1855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2274,6 +2626,326 @@
         </is>
       </c>
       <c r="F24" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:03:13</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:03:17</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>78.4%</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>14:03:22</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14:03:27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>77.9%</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:03:38</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:03:43</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:03:48</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:03:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:03:58</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:04:03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -2290,7 +2962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3061,6 +3733,326 @@
         </is>
       </c>
       <c r="F24" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>14:03:13</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14:03:18</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>14:03:23</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14:03:28</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>14:03:38</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:03:43</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:03:48</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>14:03:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14:03:58</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>14:04:03</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:05:20
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1841,6 +1841,390 @@
       <c r="F41" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>14:04:15</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:04:17</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>14:04:22</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>14:04:27</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14:04:35</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>14:04:40</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>14:04:44</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>14:04:52</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>14:04:57</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>14:05:02</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>14:05:07</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>14:05:14</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -1855,7 +2239,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2946,6 +3330,326 @@
         </is>
       </c>
       <c r="F34" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:04:16</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:04:18</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:04:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:04:38</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>14:04:48</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:04:53</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>14:04:58</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>14:05:03</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:05:08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>14:05:13</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -2962,7 +3666,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4053,6 +4757,326 @@
         </is>
       </c>
       <c r="F34" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>14:04:16</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>14:04:18</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>14:04:33</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:04:38</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>14:04:48</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:04:53</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>14:04:58</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>14:05:03</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>14:05:08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>14:05:13</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:06:26
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2223,6 +2223,422 @@
         </is>
       </c>
       <c r="F53" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>14:05:22</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>14:05:24</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>14:05:30</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>14:05:35</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>14:05:40</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>14:05:45</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>14:05:50</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>14:05:55</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>14:06:00</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>14:06:05</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>14:06:10</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>14:06:15</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>14:06:20</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -2239,7 +2655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3650,6 +4066,358 @@
         </is>
       </c>
       <c r="F44" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>14:05:23</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14:05:28</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>14:05:33</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>14:05:38</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>14:05:43</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>14:05:48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>14:05:53</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>14:05:58</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>14:06:03</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>14:06:13</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>14:06:19</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -3666,7 +4434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5077,6 +5845,358 @@
         </is>
       </c>
       <c r="F44" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>14:05:23</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>14:05:28</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>14:05:33</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>14:05:39</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>14:05:44</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>14:05:49</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>14:05:54</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>14:05:59</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>14:06:04</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>14:06:14</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>14:06:19</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:07:46
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2639,6 +2639,422 @@
         </is>
       </c>
       <c r="F66" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>14:06:29</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>14:06:30</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>14:06:30</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>14:06:38</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>14:06:39</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:06:46</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>14:06:49</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>14:06:57</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>14:07:02</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>14:07:07</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>14:07:15</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14:07:19</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>14:07:24</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -2655,7 +3071,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4418,6 +4834,230 @@
         </is>
       </c>
       <c r="F55" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>14:06:28</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>14:06:34</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>14:06:49</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>14:06:59</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>14:07:09</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>14:07:19</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>14:07:24</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -4434,7 +5074,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6197,6 +6837,230 @@
         </is>
       </c>
       <c r="F55" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>14:06:28</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>14:06:34</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>14:06:49</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>14:06:59</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>14:07:09</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>14:07:19</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>14:07:24</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:09:06
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3057,6 +3057,550 @@
       <c r="F79" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>14:07:51</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>14:07:52</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>14:07:53</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>14:07:53</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>14:07:54</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>14:07:55</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>14:07:56</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>14:08:04</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>14:08:09</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>14:08:13</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>14:08:21</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>14:08:26</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>14:08:34</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>14:08:39</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>14:08:44</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>14:08:49</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>14:08:49</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5058,6 +5602,390 @@
         </is>
       </c>
       <c r="F62" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>14:07:51</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>14:07:51</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>14:07:52</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>14:07:53</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>14:07:54</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>14:08:04</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>14:08:09</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>14:08:14</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>14:08:19</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:08:34</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>14:08:39</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>14:08:44</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -5074,7 +6002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7061,6 +7989,390 @@
         </is>
       </c>
       <c r="F62" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>14:07:51</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>14:07:52</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>14:07:52</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>14:07:53</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>14:07:54</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>14:08:04</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>14:08:09</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>14:08:14</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>14:08:20</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>14:08:34</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>14:08:40</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>14:08:45</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:10:18
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3601,6 +3601,518 @@
       <c r="F96" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>14:09:13</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>14:09:14</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>14:09:15</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>14:09:16</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>14:09:17</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>14:09:22</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>14:09:23</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>14:09:30</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>14:09:35</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>14:09:40</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>14:09:45</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>14:09:51</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>14:09:56</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>14:10:01</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>14:10:06</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>14:10:11</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -3615,7 +4127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5986,6 +6498,454 @@
         </is>
       </c>
       <c r="F74" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>14:09:13</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>14:09:14</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>77.0%</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>14:09:14</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14:09:15</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>14:09:16</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>14:09:19</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>14:09:30</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>14:09:35</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>14:09:40</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>14:09:45</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>14:09:55</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>14:10:00</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>14:10:05</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>14:10:10</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -6002,7 +6962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8373,6 +9333,454 @@
         </is>
       </c>
       <c r="F74" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>14:09:13</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>14:09:14</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>14:09:15</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14:09:16</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>14:09:17</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>14:09:20</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>14:09:30</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>14:09:35</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>14:09:40</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>14:09:45</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>14:09:55</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>14:10:00</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>14:10:05</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>14:10:10</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:11:25
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4111,6 +4111,422 @@
         </is>
       </c>
       <c r="F112" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>14:10:20</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>14:10:21</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>14:10:26</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>14:10:31</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>14:10:36</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>14:10:41</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>14:10:46</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>14:10:51</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>14:10:56</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>14:11:01</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>14:11:06</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>14:11:11</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>14:11:16</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -4127,7 +4543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6946,6 +7362,390 @@
         </is>
       </c>
       <c r="F88" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>14:10:19</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>14:10:20</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>14:10:30</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>14:10:35</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>14:10:40</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>14:10:45</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>14:10:50</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>14:10:55</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>14:11:00</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>14:11:05</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>14:11:10</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>14:11:15</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -6962,7 +7762,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9781,6 +10581,390 @@
         </is>
       </c>
       <c r="F88" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>14:10:20</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>14:10:21</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>14:10:30</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>14:10:35</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>14:10:40</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>14:10:45</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>14:10:51</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>14:10:55</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>14:11:01</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>14:11:05</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>14:11:11</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>14:11:15</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -9797,7 +10981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9834,6 +11018,102 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>14:11:12</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bathroom Door</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ENTER</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>User ENTERED Bathroom</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14:11:17</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bathroom Door</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>User EXITED Bathroom</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>14:11:19</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bathroom Door</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ENTER</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>User ENTERED Bathroom</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:12:33
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,70 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>14:12:08</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MINIMAL</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MINIMAL ALERT: Bathroom occupied, no motion &gt; 20s.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14:12:20</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MODERATE</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>MODERATE ALERT: Bathroom occupied, no motion &gt; 40s.</t>
         </is>
       </c>
     </row>
@@ -524,7 +588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4527,6 +4591,454 @@
         </is>
       </c>
       <c r="F125" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>14:11:28</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>14:11:29</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>14:11:31</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>14:11:36</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>14:11:41</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>14:11:46</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>14:11:51</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>14:11:56</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>14:12:01</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>14:12:06</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>14:12:11</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>14:12:16</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>14:12:22</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>14:12:27</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -4543,7 +5055,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7746,6 +8258,294 @@
         </is>
       </c>
       <c r="F100" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>14:11:28</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>14:11:35</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>14:11:45</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>76.5%</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>14:11:55</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>14:12:00</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>14:12:05</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>14:12:10</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>14:12:21</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>76.3%</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -7762,7 +8562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10965,6 +11765,294 @@
         </is>
       </c>
       <c r="F100" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>14:11:29</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>14:11:36</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>14:11:46</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>14:11:56</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>14:12:01</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>14:12:06</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>14:12:11</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>14:12:21</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>25.0C</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>14:12:26</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -10981,7 +12069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11112,6 +12200,70 @@
         </is>
       </c>
       <c r="F4" t="inlineStr">
+        <is>
+          <t>User ENTERED Bathroom</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14:11:29</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bathroom Door</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>EXIT</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>User EXITED Bathroom</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14:11:37</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bathroom Door</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ENTER</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>User ENTERED Bathroom</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:13:40
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +523,38 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>MODERATE ALERT: Bathroom occupied, no motion &gt; 40s.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>14:12:41</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CRITICAL</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CRITICAL ALERT: Bathroom occupied, no motion &gt; 60s.</t>
         </is>
       </c>
     </row>
@@ -588,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5039,6 +5071,422 @@
         </is>
       </c>
       <c r="F139" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>14:12:36</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>14:12:37</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>14:12:42</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>14:12:49</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>14:12:54</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>14:12:59</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>14:13:04</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>14:13:09</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>14:13:14</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>14:13:19</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>14:13:24</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>14:13:29</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>14:13:34</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -5055,7 +5503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8546,6 +8994,390 @@
         </is>
       </c>
       <c r="F109" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>14:12:35</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>14:12:36</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>76.3%</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>14:12:41</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>14:12:46</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>76.3%</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>14:12:51</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>14:12:56</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>76.2%</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>14:13:01</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>14:13:06</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>76.2%</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>14:13:16</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>76.1%</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>14:13:21</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>77.1%</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>14:13:26</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>76.1%</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>14:13:31</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>77.0%</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -8562,7 +9394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12053,6 +12885,390 @@
         </is>
       </c>
       <c r="F109" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>14:12:35</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>25.0C</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>14:12:37</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>14:12:41</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>14:12:46</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>14:12:51</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>14:12:56</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>14:13:01</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>14:13:06</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>14:13:16</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>14:13:21</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>14:13:26</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>14:13:31</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:14:47
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5487,6 +5487,390 @@
         </is>
       </c>
       <c r="F152" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>14:13:43</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>14:13:44</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>14:13:49</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>14:13:54</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>14:13:59</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>14:14:04</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>14:14:09</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>14:14:14</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>14:14:19</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>14:14:24</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>14:14:32</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>14:14:37</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -5503,7 +5887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9378,6 +9762,454 @@
         </is>
       </c>
       <c r="F121" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>14:13:42</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>14:13:43</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>14:13:46</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>76.3%</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>14:13:51</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>14:13:56</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>76.2%</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>14:14:01</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>14:14:06</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>76.3%</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>14:14:11</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>14:14:16</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>76.4%</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>14:14:21</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>14:14:26</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>14:14:31</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>14:14:36</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>14:14:41</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -9394,7 +10226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13269,6 +14101,454 @@
         </is>
       </c>
       <c r="F121" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>14:13:42</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>14:13:44</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>14:13:46</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>14:13:51</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>14:13:56</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>14:14:02</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>14:14:07</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>14:14:12</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>24.9C</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>14:14:17</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>14:14:22</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>14:14:27</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>14:14:32</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>14:14:37</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>14:14:42</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:15:53
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5871,6 +5871,422 @@
         </is>
       </c>
       <c r="F164" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>14:14:48</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>14:14:50</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>14:14:54</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14:14:59</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>14:15:04</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>14:15:13</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>14:15:18</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>14:15:22</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>14:15:28</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>14:15:28</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>14:15:35</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>14:15:38</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>14:15:45</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -5887,7 +6303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10210,6 +10626,390 @@
         </is>
       </c>
       <c r="F135" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>14:14:49</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>14:14:51</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>14:14:56</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>76.7%</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>14:15:01</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>14:15:06</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>14:15:12</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>14:15:17</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>14:15:27</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>14:15:32</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>14:15:37</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>77.0%</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>14:15:42</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>14:15:47</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>77.1%</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -10226,7 +11026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14549,6 +15349,390 @@
         </is>
       </c>
       <c r="F135" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>14:14:49</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>14:14:52</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>14:14:57</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>14:15:02</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>14:15:07</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>14:15:12</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>14:15:17</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>14:15:27</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>14:15:32</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>14:15:37</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>14:15:42</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>14:15:47</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:17:00
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F177"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6287,6 +6287,454 @@
         </is>
       </c>
       <c r="F177" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>14:15:54</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>14:15:56</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>14:15:57</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>14:16:03</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>14:16:08</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>14:16:09</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>14:16:17</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>14:16:23</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>14:16:28</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:16:32</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>14:16:39</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>14:16:44</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>14:16:49</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>14:16:54</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -6303,7 +6751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11010,6 +11458,326 @@
         </is>
       </c>
       <c r="F147" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>14:15:55</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>14:15:57</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>77.0%</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>14:16:02</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>14:16:12</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>14:16:22</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>14:16:27</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>78.3%</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>14:16:32</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>14:16:37</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>14:16:47</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>77.9%</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>14:16:52</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -11026,7 +11794,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15733,6 +16501,326 @@
         </is>
       </c>
       <c r="F147" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>14:15:55</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>14:15:58</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>14:16:02</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>14:16:12</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>14:16:22</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>14:16:27</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>14:16:33</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>14:16:38</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>14:16:48</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>14:16:53</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:18:06
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:F203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6735,6 +6735,390 @@
         </is>
       </c>
       <c r="F191" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>14:17:02</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>14:17:04</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:17:11</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>14:17:15</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>14:17:24</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>14:17:29</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:17:35</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:17:40</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:17:45</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>14:17:50</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>14:17:55</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>14:18:00</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -6751,7 +7135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11778,6 +12162,422 @@
         </is>
       </c>
       <c r="F157" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>14:17:01</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>14:17:03</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>14:17:07</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>14:17:12</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>14:17:17</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>14:17:22</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>14:17:27</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>14:17:32</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>14:17:37</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>77.9%</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>14:17:42</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>77.0%</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14:17:47</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>77.9%</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>14:17:52</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>76.8%</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>14:17:57</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -11794,7 +12594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16821,6 +17621,422 @@
         </is>
       </c>
       <c r="F157" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>14:17:02</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>24.8C</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>14:17:03</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>14:17:08</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>14:17:13</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>14:17:18</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>14:17:23</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>14:17:28</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>14:17:33</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>14:17:38</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>14:17:43</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14:17:48</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>14:17:53</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>14:17:58</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:19:13
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F203"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7119,6 +7119,422 @@
         </is>
       </c>
       <c r="F203" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>14:18:08</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:18:10</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>14:18:12</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>14:18:20</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>14:18:25</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>14:18:30</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>14:18:35</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>14:18:37</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>14:18:44</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>14:18:49</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>14:18:55</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>14:19:00</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>14:19:05</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -7135,7 +7551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12578,6 +12994,358 @@
         </is>
       </c>
       <c r="F170" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>14:18:07</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>76.9%</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>14:18:09</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>78.1%</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>14:18:13</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>14:18:18</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>78.3%</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>14:18:23</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>14:18:28</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>14:18:33</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>77.9%</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>14:18:38</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>14:18:43</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>14:18:48</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>14:18:53</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -12594,7 +13362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18037,6 +18805,358 @@
         </is>
       </c>
       <c r="F170" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>14:18:08</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>14:18:10</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>14:18:13</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>14:18:18</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>14:18:23</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>14:18:28</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>14:18:33</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>14:18:38</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>14:18:44</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>14:18:48</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>14:18:54</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:20:19
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7537,6 +7537,454 @@
       <c r="F216" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>14:19:16</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>14:19:17</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>14:19:19</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>14:19:24</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>14:19:25</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>14:19:34</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>14:19:40</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>14:19:44</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>14:19:45</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>14:19:52</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>14:19:57</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>14:20:02</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>14:20:07</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>14:20:09</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -7551,7 +7999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13346,6 +13794,422 @@
         </is>
       </c>
       <c r="F181" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>14:19:15</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>14:19:18</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>77.7%</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>14:19:23</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>14:19:28</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>14:19:33</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>78.3%</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:19:38</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>14:19:43</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>14:19:48</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>79.0%</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>14:19:53</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>14:19:58</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>80.3%</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>14:20:03</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>78.4%</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>14:20:08</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>79.3%</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:20:14</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>78.1%</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -13362,7 +14226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F181"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19157,6 +20021,422 @@
         </is>
       </c>
       <c r="F181" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>14:19:15</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>14:19:19</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>14:19:24</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>14:19:29</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>14:19:34</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>14:19:39</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>14:19:44</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>14:19:49</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>14:19:54</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>14:19:59</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>14:20:04</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>14:20:09</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>14:20:14</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:21:25
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F230"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7985,6 +7985,422 @@
       <c r="F230" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:20:21</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:20:23</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:20:27</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>14:20:32</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>14:20:37</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>14:20:42</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>14:20:47</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:20:52</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>14:20:57</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>14:21:02</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>14:21:07</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:21:12</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>14:21:17</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -7999,7 +8415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F194"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14210,6 +14626,262 @@
         </is>
       </c>
       <c r="F194" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>14:20:22</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>14:20:23</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>14:20:28</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>79.0%</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:20:33</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:20:38</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:20:43</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>14:20:59</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>14:21:09</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -14226,7 +14898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F194"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20437,6 +21109,262 @@
         </is>
       </c>
       <c r="F194" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>14:20:22</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>14:20:24</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>14:20:29</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>14:20:34</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>14:20:39</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>14:20:44</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>14:20:59</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>14:21:09</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:22:32
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F243"/>
+  <dimension ref="A1:F255"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8401,6 +8401,390 @@
       <c r="F243" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>14:21:27</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>14:21:28</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>14:21:35</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>14:21:40</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>14:21:43</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>14:21:51</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>14:21:56</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:22:01</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:22:06</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>14:22:11</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:22:16</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:22:20</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -8415,7 +8799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F202"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14882,6 +15266,326 @@
         </is>
       </c>
       <c r="F202" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>14:21:29</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>14:21:34</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>78.4%</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:21:39</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>78.3%</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>14:21:44</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>78.1%</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>14:21:49</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>14:21:54</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>14:22:04</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>14:22:09</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>14:22:19</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>14:22:24</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>78.3%</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -14898,7 +15602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F202"/>
+  <dimension ref="A1:F212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21365,6 +22069,326 @@
         </is>
       </c>
       <c r="F202" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>14:21:29</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>14:21:34</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>14:21:40</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>14:21:44</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>14:21:50</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>14:21:55</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>14:22:05</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>14:22:10</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>14:22:20</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>14:22:25</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:23:39
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8785,6 +8785,454 @@
       <c r="F255" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:22:34</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:22:36</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>14:22:38</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>14:22:43</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>14:22:48</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>14:22:51</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>14:22:58</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>14:23:03</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:23:04</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>14:23:11</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>14:23:16</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>14:23:21</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>14:23:26</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>14:23:31</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -8799,7 +9247,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:F223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15586,6 +16034,358 @@
         </is>
       </c>
       <c r="F212" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>14:22:34</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>77.5%</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>14:22:36</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>14:22:39</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>77.2%</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>14:22:44</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>78.1%</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>14:22:49</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>77.4%</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>14:22:59</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>77.3%</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>14:23:04</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>14:23:15</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>14:23:19</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>77.6%</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>14:23:25</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>14:23:29</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>77.8%</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -15602,7 +16402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:F223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22389,6 +23189,358 @@
         </is>
       </c>
       <c r="F212" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>14:22:35</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>14:22:37</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>14:22:40</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>14:22:45</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>14:22:50</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>14:23:00</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>14:23:05</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>24.7C</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>14:23:15</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>14:23:20</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>14:23:25</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>24.6C</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>14:23:30</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:24:46
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F269"/>
+  <dimension ref="A1:F283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9233,6 +9233,454 @@
       <c r="F269" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>14:23:42</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>14:23:44</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>14:23:46</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>14:23:52</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>14:23:58</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>14:24:03</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>14:24:08</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>14:24:13</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>14:24:18</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>14:24:21</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>14:24:27</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>14:24:28</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>14:24:36</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>14:24:38</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -9247,7 +9695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16386,6 +16834,422 @@
         </is>
       </c>
       <c r="F223" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>14:23:40</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>14:23:42</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>78.0%</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>14:23:45</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>79.0%</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>14:23:50</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>78.2%</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>14:23:55</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>14:24:00</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>14:24:05</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:24:10</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:24:15</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:24:20</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>14:24:25</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>14:24:30</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>14:24:40</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -16402,7 +17266,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23541,6 +24405,390 @@
         </is>
       </c>
       <c r="F223" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>14:23:41</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>14:23:43</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>14:23:45</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>24.5C</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>14:23:50</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>14:23:55</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>14:24:00</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>14:24:05</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:24:10</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:24:15</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:24:20</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>14:24:26</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>14:24:31</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:25:52
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F283"/>
+  <dimension ref="A1:F296"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9679,6 +9679,422 @@
         </is>
       </c>
       <c r="F283" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>14:24:50</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>14:24:52</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>14:24:53</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>14:25:02</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>14:25:02</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>14:25:08</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>14:25:13</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>14:25:17</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>14:25:23</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>14:25:27</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>14:25:33</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>14:25:38</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>14:25:40</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -9695,7 +10111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F236"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17250,6 +17666,294 @@
         </is>
       </c>
       <c r="F236" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>14:24:49</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:24:51</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>14:25:00</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>14:25:05</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>14:25:10</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:25:15</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>14:25:20</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>14:25:25</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>14:25:35</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -17266,7 +17970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24789,6 +25493,326 @@
         </is>
       </c>
       <c r="F235" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>14:24:48</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>14:24:49</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:24:52</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>14:25:01</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>14:25:06</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>14:25:11</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:25:16</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>14:25:21</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>14:25:26</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>14:25:36</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:26:58
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F296"/>
+  <dimension ref="A1:F311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10095,6 +10095,486 @@
         </is>
       </c>
       <c r="F296" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>14:25:54</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>14:25:55</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>14:25:57</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>14:26:01</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>14:26:03</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>14:26:12</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>14:26:13</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>14:26:19</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>14:26:24</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>14:26:29</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>14:26:34</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>14:26:39</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>14:26:44</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>14:26:49</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>14:26:52</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -10111,7 +10591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F245"/>
+  <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17954,6 +18434,294 @@
         </is>
       </c>
       <c r="F245" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>14:25:55</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>14:26:05</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>79.8%</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>14:26:10</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>14:26:15</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>14:26:30</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:26:35</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:26:41</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>14:26:46</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:26:51</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -17970,7 +18738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F245"/>
+  <dimension ref="A1:F254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25813,6 +26581,294 @@
         </is>
       </c>
       <c r="F245" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>14:25:56</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>14:26:06</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>14:26:11</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>14:26:16</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>14:26:31</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:26:36</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:26:41</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>14:26:46</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:26:51</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:28:06
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F311"/>
+  <dimension ref="A1:F323"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10577,6 +10577,390 @@
       <c r="F311" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>14:27:00</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>14:27:03</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>14:27:11</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>14:27:17</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>14:27:22</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>14:27:24</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>14:27:33</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>14:27:37</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>14:27:43</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>14:27:48</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>14:27:53</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>14:27:58</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -10591,7 +10975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F254"/>
+  <dimension ref="A1:F265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18722,6 +19106,358 @@
         </is>
       </c>
       <c r="F254" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:27:01</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:27:06</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:27:16</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>14:27:21</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>14:27:26</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>14:27:31</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>14:27:36</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>14:27:41</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>14:27:46</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:27:51</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>14:27:56</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -18738,7 +19474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F254"/>
+  <dimension ref="A1:F265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26869,6 +27605,358 @@
         </is>
       </c>
       <c r="F254" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:27:02</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:27:06</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:27:17</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>14:27:22</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>14:27:27</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>14:27:32</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>14:27:37</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>14:27:42</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>14:27:47</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>14:27:52</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>14:27:57</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:29:13
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F323"/>
+  <dimension ref="A1:F337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10959,6 +10959,454 @@
         </is>
       </c>
       <c r="F323" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>14:28:09</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>14:28:10</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>14:28:14</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>14:28:15</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>14:28:23</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>14:28:27</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>14:28:28</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>14:28:35</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>14:28:41</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>14:28:46</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>14:28:50</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>14:28:53</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>14:29:01</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>14:29:06</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -10975,7 +11423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F265"/>
+  <dimension ref="A1:F277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19458,6 +19906,390 @@
         </is>
       </c>
       <c r="F265" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>14:28:07</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>14:28:11</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>79.3%</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>14:28:16</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>14:28:21</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>79.4%</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>14:28:31</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>14:28:36</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>14:28:42</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>14:28:47</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>78.5%</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>14:28:51</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>14:28:56</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>14:29:02</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>14:29:07</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -19474,7 +20306,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F265"/>
+  <dimension ref="A1:F276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27957,6 +28789,358 @@
         </is>
       </c>
       <c r="F265" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>14:28:08</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>14:28:12</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>14:28:17</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>14:28:22</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>14:28:32</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>14:28:37</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>14:28:42</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>14:28:47</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>14:28:52</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>14:28:57</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>14:29:02</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:30:21
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F337"/>
+  <dimension ref="A1:F349"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11407,6 +11407,390 @@
         </is>
       </c>
       <c r="F337" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>14:29:15</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>14:29:17</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>14:29:21</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>14:29:25</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>14:29:34</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>14:29:39</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>14:29:43</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>14:29:50</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F345" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>14:29:54</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>14:30:10</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F347" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>14:30:11</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F348" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>14:30:14</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F349" t="inlineStr">
         <is>
           <t>Inactive</t>
         </is>
@@ -11423,7 +11807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F277"/>
+  <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20290,6 +20674,326 @@
         </is>
       </c>
       <c r="F277" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>14:29:16</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>14:29:18</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>14:29:21</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>14:29:26</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>14:29:32</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>14:29:37</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>14:29:42</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>14:29:47</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>14:30:08</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>14:30:12</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -20306,7 +21010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F276"/>
+  <dimension ref="A1:F287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29141,6 +29845,358 @@
         </is>
       </c>
       <c r="F276" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>14:29:14</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>14:29:17</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>14:29:19</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>14:29:22</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>14:29:27</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>14:29:33</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>14:29:38</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>14:29:42</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>14:29:48</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>14:30:09</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>14:30:13</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:31:29
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F349"/>
+  <dimension ref="A1:F365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11793,6 +11793,518 @@
       <c r="F349" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>14:30:25</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F350" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>14:30:26</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>14:30:27</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>14:30:30</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>14:30:30</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>14:30:38</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>14:30:43</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>14:30:48</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>14:30:54</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F358" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>14:30:58</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F359" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>14:30:59</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>14:31:09</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>14:31:14</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>14:31:19</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>14:31:22</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>14:31:23</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -11807,7 +12319,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F287"/>
+  <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20994,6 +21506,262 @@
         </is>
       </c>
       <c r="F287" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>14:30:23</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>14:30:28</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>14:30:32</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>14:30:52</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>14:31:02</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>79.5%</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>14:31:07</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>79.7%</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>14:31:12</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>14:31:17</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -21010,7 +21778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F287"/>
+  <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30197,6 +30965,262 @@
         </is>
       </c>
       <c r="F287" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>14:30:24</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>14:30:29</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>14:30:33</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>24.4C</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>14:30:53</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>14:31:03</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>14:31:08</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>14:31:13</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>14:31:18</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:32:36
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F365"/>
+  <dimension ref="A1:F378"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12303,6 +12303,422 @@
         </is>
       </c>
       <c r="F365" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>14:31:33</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>14:31:35</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>14:31:40</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>14:31:45</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F369" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>14:31:50</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>14:31:55</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F371" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>14:32:00</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F372" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>14:32:09</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>14:32:10</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>14:32:16</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>14:32:21</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>14:32:26</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>14:32:27</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -12319,7 +12735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F295"/>
+  <dimension ref="A1:F307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21762,6 +22178,390 @@
         </is>
       </c>
       <c r="F295" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>14:31:31</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>14:31:34</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>14:31:37</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>14:31:42</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>14:31:47</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>14:31:52</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>14:31:57</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>14:32:02</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>14:32:07</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>14:32:12</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>14:32:17</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>14:32:23</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>78.9%</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -21778,7 +22578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F295"/>
+  <dimension ref="A1:F307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31221,6 +32021,390 @@
         </is>
       </c>
       <c r="F295" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>14:31:32</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>14:31:35</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>14:31:38</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>14:31:43</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>14:31:48</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>14:31:53</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>14:31:58</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>14:32:03</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>14:32:08</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>14:32:13</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>14:32:18</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>14:32:23</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:33:43
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F378"/>
+  <dimension ref="A1:F392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12719,6 +12719,454 @@
         </is>
       </c>
       <c r="F378" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>14:32:39</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>14:32:42</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>14:32:44</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>14:32:50</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>14:32:55</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>14:33:00</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>14:33:06</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>14:33:10</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>14:33:16</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>14:33:17</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>14:33:25</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>14:33:27</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>14:33:35</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>14:33:36</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -12735,7 +13183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F307"/>
+  <dimension ref="A1:F319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22562,6 +23010,390 @@
         </is>
       </c>
       <c r="F307" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>14:32:37</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>14:32:40</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>14:32:48</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>79.8%</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>14:32:53</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>14:32:58</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>14:33:03</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>14:33:08</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>14:33:13</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>78.6%</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>14:33:18</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>14:33:23</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>78.7%</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>14:33:28</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>79.6%</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>14:33:33</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>78.8%</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -22578,7 +23410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F307"/>
+  <dimension ref="A1:F319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32405,6 +33237,390 @@
         </is>
       </c>
       <c r="F307" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>14:32:38</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>14:32:41</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>14:32:49</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>14:32:54</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>14:32:59</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>14:33:04</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>14:33:09</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>14:33:14</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>14:33:19</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>14:33:24</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>14:33:29</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>14:33:34</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:34:50
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F392"/>
+  <dimension ref="A1:F404"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13169,6 +13169,390 @@
       <c r="F392" t="inlineStr">
         <is>
           <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>14:33:48</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F393" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>14:33:51</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>14:33:52</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>14:33:58</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>14:34:03</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>14:34:08</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>14:34:13</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>14:34:16</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>14:34:25</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>14:34:30</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>14:34:31</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>14:34:41</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>Inactive</t>
         </is>
       </c>
     </row>
@@ -13183,7 +13567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23394,6 +23778,422 @@
         </is>
       </c>
       <c r="F319" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>14:33:44</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>79.8%</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>14:33:46</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>79.0%</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>14:33:49</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>14:33:53</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>14:33:58</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>14:34:03</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>79.0%</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>14:34:08</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>79.9%</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>14:34:18</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>14:34:23</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>14:34:28</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>80.2%</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>14:34:33</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>14:34:38</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>14:34:43</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>79.3%</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -23410,7 +24210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33621,6 +34421,422 @@
         </is>
       </c>
       <c r="F319" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>14:33:45</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>14:33:47</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>24.3C</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>14:33:50</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>14:33:54</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>14:34:00</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>14:34:04</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>14:34:10</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>14:34:19</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>14:34:24</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>14:34:29</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>14:34:34</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>14:34:39</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>14:34:44</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>

<commit_message>
Auto update Excel log 2026-02-04 14:35:56
</commit_message>
<xml_diff>
--- a/SeniorConnect_MasterLog.xlsx
+++ b/SeniorConnect_MasterLog.xlsx
@@ -620,7 +620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F404"/>
+  <dimension ref="A1:F418"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13553,6 +13553,454 @@
       <c r="F404" t="inlineStr">
         <is>
           <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>14:34:51</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>14:34:52</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>14:34:55</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>14:34:58</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>14:35:02</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>14:35:07</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>14:35:12</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>14:35:16</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>14:35:24</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>14:35:25</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>14:35:32</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>14:35:36</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>14:35:46</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>No Motion</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>14:35:47</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>Motion Detected</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -13567,7 +14015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F332"/>
+  <dimension ref="A1:F340"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24194,6 +24642,262 @@
         </is>
       </c>
       <c r="F332" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>14:34:53</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>80.2%</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>14:34:56</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>79.2%</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>14:35:08</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>14:35:19</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>79.1%</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>14:35:29</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>14:35:39</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>78.4%</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>14:35:44</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>14:35:49</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>80.0%</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
@@ -24210,7 +24914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F332"/>
+  <dimension ref="A1:F340"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34837,6 +35541,262 @@
         </is>
       </c>
       <c r="F332" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>14:34:54</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>14:34:57</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>14:35:09</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>14:35:20</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>14:35:30</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F337" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>14:35:40</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>14:35:45</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>14:35:50</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Bathroom</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>24.2C</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
         <is>
           <t>Active</t>
         </is>

</xml_diff>